<commit_message>
admin transaction data verify updated
admin transaction data verify updated
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>normaltester</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>3346685184</t>
+  </si>
+  <si>
+    <t>3373363968</t>
+  </si>
+  <si>
+    <t>3367494400</t>
+  </si>
+  <si>
+    <t>3315788544</t>
   </si>
 </sst>
 </file>
@@ -432,6 +441,21 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Members List widget started
Members List widget started
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>normaltester</t>
   </si>
@@ -67,6 +67,45 @@
   </si>
   <si>
     <t>3315788544</t>
+  </si>
+  <si>
+    <t>3307523712</t>
+  </si>
+  <si>
+    <t>3330617856</t>
+  </si>
+  <si>
+    <t>3395766528</t>
+  </si>
+  <si>
+    <t>3363618368</t>
+  </si>
+  <si>
+    <t>3347262720</t>
+  </si>
+  <si>
+    <t>3341588992</t>
+  </si>
+  <si>
+    <t>3301434112</t>
+  </si>
+  <si>
+    <t>3378266880</t>
+  </si>
+  <si>
+    <t>3310577920</t>
+  </si>
+  <si>
+    <t>3312903936</t>
+  </si>
+  <si>
+    <t>3341903360</t>
+  </si>
+  <si>
+    <t>3353564160</t>
+  </si>
+  <si>
+    <t>3306600448</t>
   </si>
 </sst>
 </file>
@@ -456,6 +495,71 @@
         <v>16</v>
       </c>
     </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Adyen, setDefaultState, reorganized project structure
Added Adyen, setDefaultState, reorganized project structure
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>normaltester</t>
   </si>
@@ -109,6 +109,63 @@
   </si>
   <si>
     <t>3397079808</t>
+  </si>
+  <si>
+    <t>3320036608</t>
+  </si>
+  <si>
+    <t>3318789888</t>
+  </si>
+  <si>
+    <t>3335400448</t>
+  </si>
+  <si>
+    <t>3386408704</t>
+  </si>
+  <si>
+    <t>3373721088</t>
+  </si>
+  <si>
+    <t>3301729792</t>
+  </si>
+  <si>
+    <t>3309341952</t>
+  </si>
+  <si>
+    <t>3353609728</t>
+  </si>
+  <si>
+    <t>3311197184</t>
+  </si>
+  <si>
+    <t>3392648960</t>
+  </si>
+  <si>
+    <t>3385755136</t>
+  </si>
+  <si>
+    <t>3340498176</t>
+  </si>
+  <si>
+    <t>3389296640</t>
+  </si>
+  <si>
+    <t>3319841000</t>
+  </si>
+  <si>
+    <t>3335292672</t>
+  </si>
+  <si>
+    <t>YOUR PAYMENT WAS DECLINED</t>
+  </si>
+  <si>
+    <t>3399858176</t>
+  </si>
+  <si>
+    <t>3388921856</t>
+  </si>
+  <si>
+    <t>3397952512</t>
   </si>
 </sst>
 </file>
@@ -568,6 +625,102 @@
         <v>30</v>
       </c>
     </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed some excel issues, transactionFragment is now common class
Fixed some excel issues, transactionFragment is now common class
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,9 +16,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>3302397440</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+  <si>
+    <t>3399320032</t>
+  </si>
+  <si>
+    <t>3316570112</t>
+  </si>
+  <si>
+    <t>3343357696</t>
+  </si>
+  <si>
+    <t>3322302976</t>
+  </si>
+  <si>
+    <t>3332153472</t>
+  </si>
+  <si>
+    <t>3392621184</t>
+  </si>
+  <si>
+    <t>3355435520</t>
+  </si>
+  <si>
+    <t>3346247168</t>
+  </si>
+  <si>
+    <t>3361960704</t>
+  </si>
+  <si>
+    <t>YOUR PAYMENT WAS DECLINED</t>
+  </si>
+  <si>
+    <t>3397409792</t>
+  </si>
+  <si>
+    <t>3328901632</t>
+  </si>
+  <si>
+    <t>3371851520</t>
+  </si>
+  <si>
+    <t>3311340544</t>
+  </si>
+  <si>
+    <t>3338834688</t>
+  </si>
+  <si>
+    <t>3334672128</t>
+  </si>
+  <si>
+    <t>3361707520</t>
+  </si>
+  <si>
+    <t>3321968266</t>
+  </si>
+  <si>
+    <t>3341655808</t>
+  </si>
+  <si>
+    <t>3359681024</t>
+  </si>
+  <si>
+    <t>3336408064</t>
+  </si>
+  <si>
+    <t>3339858688</t>
+  </si>
+  <si>
+    <t>3381906176</t>
+  </si>
+  <si>
+    <t>3388346880</t>
+  </si>
+  <si>
+    <t>3335325696</t>
+  </si>
+  <si>
+    <t>3386407168</t>
+  </si>
+  <si>
+    <t>3357847552</t>
+  </si>
+  <si>
+    <t>3335478144</t>
+  </si>
+  <si>
+    <t>3364033536</t>
+  </si>
+  <si>
+    <t>3326515712</t>
+  </si>
+  <si>
+    <t>3338583552</t>
+  </si>
+  <si>
+    <t>3314734080</t>
+  </si>
+  <si>
+    <t>3389340544</t>
+  </si>
+  <si>
+    <t>3376333824</t>
+  </si>
+  <si>
+    <t>3353421888</t>
+  </si>
+  <si>
+    <t>3378081024</t>
+  </si>
+  <si>
+    <t>3377704192</t>
+  </si>
+  <si>
+    <t>3354159072</t>
+  </si>
+  <si>
+    <t>3310070016</t>
+  </si>
+  <si>
+    <t>3375197440</t>
   </si>
 </sst>
 </file>
@@ -361,7 +478,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,13 +486,7 @@
     <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated according to deals parameters
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="199">
   <si>
     <t>NormalTester</t>
   </si>
@@ -592,6 +592,27 @@
   </si>
   <si>
     <t>3382423744</t>
+  </si>
+  <si>
+    <t>3268.69</t>
+  </si>
+  <si>
+    <t>3304694784</t>
+  </si>
+  <si>
+    <t>3333269248</t>
+  </si>
+  <si>
+    <t>4938.98</t>
+  </si>
+  <si>
+    <t>3333494272</t>
+  </si>
+  <si>
+    <t>5098.97</t>
+  </si>
+  <si>
+    <t>3388028672</t>
   </si>
 </sst>
 </file>
@@ -948,39 +969,19 @@
         <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
USD transactions suite added
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="219">
   <si>
     <t>NormalTester</t>
   </si>
@@ -613,6 +613,66 @@
   </si>
   <si>
     <t>3388028672</t>
+  </si>
+  <si>
+    <t>5258.98</t>
+  </si>
+  <si>
+    <t>3371096320</t>
+  </si>
+  <si>
+    <t>5418.97</t>
+  </si>
+  <si>
+    <t>1321.52</t>
+  </si>
+  <si>
+    <t>3381950720</t>
+  </si>
+  <si>
+    <t>1452.77</t>
+  </si>
+  <si>
+    <t>3336102144</t>
+  </si>
+  <si>
+    <t>1584.02</t>
+  </si>
+  <si>
+    <t>3315692480</t>
+  </si>
+  <si>
+    <t>1715.27</t>
+  </si>
+  <si>
+    <t>3305644544</t>
+  </si>
+  <si>
+    <t>1846.52</t>
+  </si>
+  <si>
+    <t>3382319616</t>
+  </si>
+  <si>
+    <t>1977.77</t>
+  </si>
+  <si>
+    <t>3362865664</t>
+  </si>
+  <si>
+    <t>3330600960</t>
+  </si>
+  <si>
+    <t>2109.02</t>
+  </si>
+  <si>
+    <t>3320605440</t>
+  </si>
+  <si>
+    <t>2240.27</t>
+  </si>
+  <si>
+    <t>3322910208</t>
   </si>
 </sst>
 </file>
@@ -966,22 +1026,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
-        <v>198</v>
+      <c r="F2" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates for Successful payments visa globalcollect, chrome updates, pom updated
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="413">
   <si>
     <t>NormalTester</t>
   </si>
@@ -1039,6 +1039,222 @@
   </si>
   <si>
     <t>1717.39</t>
+  </si>
+  <si>
+    <t>iuliia.3</t>
+  </si>
+  <si>
+    <t>3352830976</t>
+  </si>
+  <si>
+    <t>3334454016</t>
+  </si>
+  <si>
+    <t>189.36</t>
+  </si>
+  <si>
+    <t>3380646912</t>
+  </si>
+  <si>
+    <t>660.91</t>
+  </si>
+  <si>
+    <t>3327241472</t>
+  </si>
+  <si>
+    <t>56.15</t>
+  </si>
+  <si>
+    <t>3368612608</t>
+  </si>
+  <si>
+    <t>1678.73</t>
+  </si>
+  <si>
+    <t>3308783360</t>
+  </si>
+  <si>
+    <t>5399.67</t>
+  </si>
+  <si>
+    <t>3359951360</t>
+  </si>
+  <si>
+    <t>14584.28</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>3314229328</t>
+  </si>
+  <si>
+    <t>199.36</t>
+  </si>
+  <si>
+    <t>750.74</t>
+  </si>
+  <si>
+    <t>60.15</t>
+  </si>
+  <si>
+    <t>1897.04</t>
+  </si>
+  <si>
+    <t>3372832000</t>
+  </si>
+  <si>
+    <t>3392461568</t>
+  </si>
+  <si>
+    <t>287.52</t>
+  </si>
+  <si>
+    <t>3371001216</t>
+  </si>
+  <si>
+    <t>735.25</t>
+  </si>
+  <si>
+    <t>3347847168</t>
+  </si>
+  <si>
+    <t>63.42</t>
+  </si>
+  <si>
+    <t>3308438016</t>
+  </si>
+  <si>
+    <t>2105.35</t>
+  </si>
+  <si>
+    <t>3325735680</t>
+  </si>
+  <si>
+    <t>5790.55</t>
+  </si>
+  <si>
+    <t>3365369600</t>
+  </si>
+  <si>
+    <t>2654.76</t>
+  </si>
+  <si>
+    <t>3308594432</t>
+  </si>
+  <si>
+    <t>301.52</t>
+  </si>
+  <si>
+    <t>824.08</t>
+  </si>
+  <si>
+    <t>67.42</t>
+  </si>
+  <si>
+    <t>2313.64</t>
+  </si>
+  <si>
+    <t>6200.83</t>
+  </si>
+  <si>
+    <t>2767.41</t>
+  </si>
+  <si>
+    <t>315.52</t>
+  </si>
+  <si>
+    <t>329.52</t>
+  </si>
+  <si>
+    <t>3348859392</t>
+  </si>
+  <si>
+    <t>357.52</t>
+  </si>
+  <si>
+    <t>371.52</t>
+  </si>
+  <si>
+    <t>3376005339</t>
+  </si>
+  <si>
+    <t>3306281175</t>
+  </si>
+  <si>
+    <t>70.69</t>
+  </si>
+  <si>
+    <t>3373696546</t>
+  </si>
+  <si>
+    <t>3318716612</t>
+  </si>
+  <si>
+    <t>74.68</t>
+  </si>
+  <si>
+    <t>3388898189</t>
+  </si>
+  <si>
+    <t>2521.94</t>
+  </si>
+  <si>
+    <t>3353686220</t>
+  </si>
+  <si>
+    <t>3355506230</t>
+  </si>
+  <si>
+    <t>6358.69</t>
+  </si>
+  <si>
+    <t>3340162017</t>
+  </si>
+  <si>
+    <t>2908.32</t>
+  </si>
+  <si>
+    <t>3357642259</t>
+  </si>
+  <si>
+    <t>399.52</t>
+  </si>
+  <si>
+    <t>413.52</t>
+  </si>
+  <si>
+    <t>961.74</t>
+  </si>
+  <si>
+    <t>427.52</t>
+  </si>
+  <si>
+    <t>3341297037</t>
+  </si>
+  <si>
+    <t>81.95</t>
+  </si>
+  <si>
+    <t>3337332298</t>
+  </si>
+  <si>
+    <t>2730.25</t>
+  </si>
+  <si>
+    <t>3336089182</t>
+  </si>
+  <si>
+    <t>6768.98</t>
+  </si>
+  <si>
+    <t>3309999836</t>
+  </si>
+  <si>
+    <t>3020.98</t>
+  </si>
+  <si>
+    <t>3370312014</t>
   </si>
 </sst>
 </file>
@@ -1395,19 +1611,19 @@
         <v>224</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>299</v>
+        <v>363</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>300</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2">
@@ -1415,10 +1631,10 @@
         <v>227</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>301</v>
+        <v>365</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -1427,7 +1643,7 @@
         <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>302</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3">
@@ -1438,7 +1654,7 @@
         <v>229</v>
       </c>
       <c r="C3" t="s">
-        <v>303</v>
+        <v>367</v>
       </c>
       <c r="D3" t="s">
         <v>231</v>
@@ -1447,7 +1663,7 @@
         <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>304</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4">
@@ -1458,7 +1674,7 @@
         <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>305</v>
+        <v>369</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -1467,7 +1683,7 @@
         <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>306</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5">
@@ -1475,19 +1691,19 @@
         <v>246</v>
       </c>
       <c r="B5" t="s">
-        <v>247</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>307</v>
+        <v>371</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
         <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>308</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6">
@@ -1495,19 +1711,19 @@
         <v>246</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
-        <v>309</v>
+        <v>373</v>
       </c>
       <c r="D6" t="s">
-        <v>251</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>310</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7">
@@ -1515,19 +1731,16 @@
         <v>224</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>311</v>
+        <v>375</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
         <v>98</v>
-      </c>
-      <c r="F7" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="8">
@@ -1535,19 +1748,16 @@
         <v>227</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>313</v>
+        <v>376</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>48</v>
-      </c>
-      <c r="F8" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="9">
@@ -1558,7 +1768,7 @@
         <v>229</v>
       </c>
       <c r="C9" t="s">
-        <v>315</v>
+        <v>377</v>
       </c>
       <c r="D9" t="s">
         <v>231</v>
@@ -1575,16 +1785,13 @@
         <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>316</v>
+        <v>378</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>98</v>
-      </c>
-      <c r="F10" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="11">
@@ -1592,19 +1799,16 @@
         <v>246</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>318</v>
+        <v>379</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="12">
@@ -1612,19 +1816,16 @@
         <v>246</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>277</v>
       </c>
       <c r="C12" t="s">
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="D12" t="s">
-        <v>251</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>72</v>
-      </c>
-      <c r="F12" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="13">
@@ -1635,7 +1836,7 @@
         <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>322</v>
+        <v>381</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1643,28 +1844,25 @@
       <c r="E13" t="s">
         <v>98</v>
       </c>
-      <c r="F13" t="s">
-        <v>323</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>324</v>
+        <v>382</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>325</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15">
@@ -1672,119 +1870,104 @@
         <v>227</v>
       </c>
       <c r="B15" t="s">
-        <v>229</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>326</v>
+        <v>376</v>
       </c>
       <c r="D15" t="s">
-        <v>231</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" t="s">
-        <v>327</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>328</v>
+        <v>382</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
         <v>98</v>
       </c>
-      <c r="F16" t="s">
-        <v>329</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>330</v>
+        <v>384</v>
       </c>
       <c r="D17" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" t="s">
-        <v>331</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s">
-        <v>277</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>332</v>
+        <v>384</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" t="s">
-        <v>333</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>334</v>
+        <v>376</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
-      </c>
-      <c r="F19" t="s">
-        <v>335</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>336</v>
+        <v>385</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="F20" t="s">
-        <v>337</v>
+        <v>386</v>
       </c>
     </row>
     <row r="21">
@@ -1792,36 +1975,344 @@
         <v>227</v>
       </c>
       <c r="B21" t="s">
-        <v>229</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>338</v>
+        <v>376</v>
       </c>
       <c r="D21" t="s">
-        <v>231</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>339</v>
+        <v>387</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B22" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" t="s">
+        <v>388</v>
+      </c>
+      <c r="D22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
         <v>232</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C22" t="s">
-        <v>340</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
+        <v>378</v>
+      </c>
+      <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>227</v>
+      </c>
+      <c r="B24" t="s">
+        <v>229</v>
+      </c>
+      <c r="C24" t="s">
+        <v>391</v>
+      </c>
+      <c r="D24" t="s">
+        <v>231</v>
+      </c>
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>232</v>
+      </c>
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>393</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>379</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>246</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>396</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B28" t="s">
+        <v>277</v>
+      </c>
+      <c r="C28" t="s">
+        <v>398</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>224</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>224</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
+        <v>401</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>227</v>
+      </c>
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" t="s">
+        <v>402</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>224</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>403</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>224</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>403</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" t="s">
+        <v>402</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>227</v>
+      </c>
+      <c r="B35" t="s">
+        <v>229</v>
+      </c>
+      <c r="C35" t="s">
+        <v>405</v>
+      </c>
+      <c r="D35" t="s">
+        <v>231</v>
+      </c>
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>232</v>
+      </c>
+      <c r="B36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" t="s">
+        <v>407</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>246</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" t="s">
+        <v>409</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>246</v>
+      </c>
+      <c r="B38" t="s">
+        <v>277</v>
+      </c>
+      <c r="C38" t="s">
+        <v>411</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Normal Account Deals first part finished
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="300">
   <si>
     <t>10</t>
   </si>
@@ -613,6 +613,309 @@
   </si>
   <si>
     <t>119.92</t>
+  </si>
+  <si>
+    <t>503.09</t>
+  </si>
+  <si>
+    <t>3338068263</t>
+  </si>
+  <si>
+    <t>513.08997</t>
+  </si>
+  <si>
+    <t>513.09</t>
+  </si>
+  <si>
+    <t>2287.47</t>
+  </si>
+  <si>
+    <t>3379237016</t>
+  </si>
+  <si>
+    <t>2327.47</t>
+  </si>
+  <si>
+    <t>2327.42</t>
+  </si>
+  <si>
+    <t>186.47</t>
+  </si>
+  <si>
+    <t>3300526535</t>
+  </si>
+  <si>
+    <t>190.47</t>
+  </si>
+  <si>
+    <t>190.5</t>
+  </si>
+  <si>
+    <t>3340370729</t>
+  </si>
+  <si>
+    <t>6064.75</t>
+  </si>
+  <si>
+    <t>6063.59</t>
+  </si>
+  <si>
+    <t>12234.49</t>
+  </si>
+  <si>
+    <t>3346149314</t>
+  </si>
+  <si>
+    <t>12409.49</t>
+  </si>
+  <si>
+    <t>12409.33</t>
+  </si>
+  <si>
+    <t>32318.23</t>
+  </si>
+  <si>
+    <t>3347285761</t>
+  </si>
+  <si>
+    <t>32818.23</t>
+  </si>
+  <si>
+    <t>3307125623</t>
+  </si>
+  <si>
+    <t>523.09</t>
+  </si>
+  <si>
+    <t>2377.73</t>
+  </si>
+  <si>
+    <t>3303409732</t>
+  </si>
+  <si>
+    <t>2417.73</t>
+  </si>
+  <si>
+    <t>2417.67</t>
+  </si>
+  <si>
+    <t>193.71</t>
+  </si>
+  <si>
+    <t>197.71</t>
+  </si>
+  <si>
+    <t>3376155468</t>
+  </si>
+  <si>
+    <t>6273.59</t>
+  </si>
+  <si>
+    <t>6272.44</t>
+  </si>
+  <si>
+    <t>12601.32</t>
+  </si>
+  <si>
+    <t>3314222351</t>
+  </si>
+  <si>
+    <t>12776.32</t>
+  </si>
+  <si>
+    <t>12776.16</t>
+  </si>
+  <si>
+    <t>33273.58</t>
+  </si>
+  <si>
+    <t>3366974200</t>
+  </si>
+  <si>
+    <t>33773.58</t>
+  </si>
+  <si>
+    <t>718.36</t>
+  </si>
+  <si>
+    <t>3302938277</t>
+  </si>
+  <si>
+    <t>732.36</t>
+  </si>
+  <si>
+    <t>2367.78</t>
+  </si>
+  <si>
+    <t>3353413515</t>
+  </si>
+  <si>
+    <t>2407.78</t>
+  </si>
+  <si>
+    <t>196.98</t>
+  </si>
+  <si>
+    <t>334303291</t>
+  </si>
+  <si>
+    <t>200.98</t>
+  </si>
+  <si>
+    <t>201.01</t>
+  </si>
+  <si>
+    <t>3389312472</t>
+  </si>
+  <si>
+    <t>6482.44</t>
+  </si>
+  <si>
+    <t>6481.27</t>
+  </si>
+  <si>
+    <t>12901.37</t>
+  </si>
+  <si>
+    <t>3337587818</t>
+  </si>
+  <si>
+    <t>13061.37</t>
+  </si>
+  <si>
+    <t>13060.6</t>
+  </si>
+  <si>
+    <t>5828.91</t>
+  </si>
+  <si>
+    <t>3391079262</t>
+  </si>
+  <si>
+    <t>5953.91</t>
+  </si>
+  <si>
+    <t>5941.62</t>
+  </si>
+  <si>
+    <t>3350852955</t>
+  </si>
+  <si>
+    <t>746.36</t>
+  </si>
+  <si>
+    <t>2457.05</t>
+  </si>
+  <si>
+    <t>3389937558</t>
+  </si>
+  <si>
+    <t>2497.05</t>
+  </si>
+  <si>
+    <t>2497.06</t>
+  </si>
+  <si>
+    <t>204.28</t>
+  </si>
+  <si>
+    <t>3355441079</t>
+  </si>
+  <si>
+    <t>208.28</t>
+  </si>
+  <si>
+    <t>208.31</t>
+  </si>
+  <si>
+    <t>3334416129</t>
+  </si>
+  <si>
+    <t>6691.27</t>
+  </si>
+  <si>
+    <t>6690.12</t>
+  </si>
+  <si>
+    <t>13313.14</t>
+  </si>
+  <si>
+    <t>3389932650</t>
+  </si>
+  <si>
+    <t>13473.14</t>
+  </si>
+  <si>
+    <t>13472.36</t>
+  </si>
+  <si>
+    <t>6012.68</t>
+  </si>
+  <si>
+    <t>3379664997</t>
+  </si>
+  <si>
+    <t>6137.68</t>
+  </si>
+  <si>
+    <t>6125.39</t>
+  </si>
+  <si>
+    <t>3378514745</t>
+  </si>
+  <si>
+    <t>760.36</t>
+  </si>
+  <si>
+    <t>760.28</t>
+  </si>
+  <si>
+    <t>2546.33</t>
+  </si>
+  <si>
+    <t>3354676935</t>
+  </si>
+  <si>
+    <t>2586.33</t>
+  </si>
+  <si>
+    <t>211.58</t>
+  </si>
+  <si>
+    <t>3325016651</t>
+  </si>
+  <si>
+    <t>215.58</t>
+  </si>
+  <si>
+    <t>215.62</t>
+  </si>
+  <si>
+    <t>3314999831</t>
+  </si>
+  <si>
+    <t>6900.12</t>
+  </si>
+  <si>
+    <t>6898.95</t>
+  </si>
+  <si>
+    <t>13724.9</t>
+  </si>
+  <si>
+    <t>3302739219</t>
+  </si>
+  <si>
+    <t>13884.9</t>
+  </si>
+  <si>
+    <t>3328210013</t>
+  </si>
+  <si>
+    <t>6250.39</t>
+  </si>
+  <si>
+    <t>6238.11</t>
   </si>
 </sst>
 </file>
@@ -963,290 +1266,7 @@
     <col min="1" max="2" width="16.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="27.28515625" collapsed="true"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>191</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>191</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>192</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" t="s">
-        <v>193</v>
-      </c>
-      <c r="G14" t="s">
-        <v>194</v>
-      </c>
-      <c r="H14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>195</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s">
-        <v>196</v>
-      </c>
-      <c r="G15" t="s">
-        <v>197</v>
-      </c>
-      <c r="H15" t="s">
-        <v>198</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
drivers moved to project folder
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="358">
   <si>
     <t>KWD</t>
   </si>
@@ -844,6 +844,252 @@
   </si>
   <si>
     <t>3375841887</t>
+  </si>
+  <si>
+    <t>3333753609</t>
+  </si>
+  <si>
+    <t>3334202470</t>
+  </si>
+  <si>
+    <t>3399066180</t>
+  </si>
+  <si>
+    <t>3358109517</t>
+  </si>
+  <si>
+    <t>210.0</t>
+  </si>
+  <si>
+    <t>3381930175</t>
+  </si>
+  <si>
+    <t>3306792453</t>
+  </si>
+  <si>
+    <t>3369586302</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>3362472968</t>
+  </si>
+  <si>
+    <t>420.0</t>
+  </si>
+  <si>
+    <t>38025.03</t>
+  </si>
+  <si>
+    <t>3342276487</t>
+  </si>
+  <si>
+    <t>38200.03</t>
+  </si>
+  <si>
+    <t>38199.94</t>
+  </si>
+  <si>
+    <t>99485.96</t>
+  </si>
+  <si>
+    <t>3323739705</t>
+  </si>
+  <si>
+    <t>99985.93</t>
+  </si>
+  <si>
+    <t>3339014984</t>
+  </si>
+  <si>
+    <t>100486.25</t>
+  </si>
+  <si>
+    <t>3337963529</t>
+  </si>
+  <si>
+    <t>100986.25</t>
+  </si>
+  <si>
+    <t>100986.22</t>
+  </si>
+  <si>
+    <t>3315144745</t>
+  </si>
+  <si>
+    <t>179.85</t>
+  </si>
+  <si>
+    <t>3329943515</t>
+  </si>
+  <si>
+    <t>219.85</t>
+  </si>
+  <si>
+    <t>17.61</t>
+  </si>
+  <si>
+    <t>3369982417</t>
+  </si>
+  <si>
+    <t>21.61</t>
+  </si>
+  <si>
+    <t>420</t>
+  </si>
+  <si>
+    <t>3325455265</t>
+  </si>
+  <si>
+    <t>630.0</t>
+  </si>
+  <si>
+    <t>38776</t>
+  </si>
+  <si>
+    <t>3397636624</t>
+  </si>
+  <si>
+    <t>38951.0</t>
+  </si>
+  <si>
+    <t>38950.92</t>
+  </si>
+  <si>
+    <t>101441.76</t>
+  </si>
+  <si>
+    <t>3324200528</t>
+  </si>
+  <si>
+    <t>101941.76</t>
+  </si>
+  <si>
+    <t>101941.72</t>
+  </si>
+  <si>
+    <t>3336774126</t>
+  </si>
+  <si>
+    <t>264.21</t>
+  </si>
+  <si>
+    <t>3362518051</t>
+  </si>
+  <si>
+    <t>304.21</t>
+  </si>
+  <si>
+    <t>24.89</t>
+  </si>
+  <si>
+    <t>28.89</t>
+  </si>
+  <si>
+    <t>630</t>
+  </si>
+  <si>
+    <t>3309155197</t>
+  </si>
+  <si>
+    <t>840.0</t>
+  </si>
+  <si>
+    <t>38941.32</t>
+  </si>
+  <si>
+    <t>3317205756</t>
+  </si>
+  <si>
+    <t>39101.32</t>
+  </si>
+  <si>
+    <t>39101.43</t>
+  </si>
+  <si>
+    <t>17450.87</t>
+  </si>
+  <si>
+    <t>17575.87</t>
+  </si>
+  <si>
+    <t>3354129786</t>
+  </si>
+  <si>
+    <t>69.2</t>
+  </si>
+  <si>
+    <t>3325088319</t>
+  </si>
+  <si>
+    <t>344.21</t>
+  </si>
+  <si>
+    <t>28.16</t>
+  </si>
+  <si>
+    <t>3313456880</t>
+  </si>
+  <si>
+    <t>32.16</t>
+  </si>
+  <si>
+    <t>840</t>
+  </si>
+  <si>
+    <t>3384860085</t>
+  </si>
+  <si>
+    <t>1050.0</t>
+  </si>
+  <si>
+    <t>3323988613</t>
+  </si>
+  <si>
+    <t>39261.43</t>
+  </si>
+  <si>
+    <t>39261.39</t>
+  </si>
+  <si>
+    <t>17522.27</t>
+  </si>
+  <si>
+    <t>3337517038</t>
+  </si>
+  <si>
+    <t>17647.27</t>
+  </si>
+  <si>
+    <t>17647.23</t>
+  </si>
+  <si>
+    <t>83.2</t>
+  </si>
+  <si>
+    <t>393.1</t>
+  </si>
+  <si>
+    <t>433.1</t>
+  </si>
+  <si>
+    <t>397.1</t>
+  </si>
+  <si>
+    <t>1050</t>
+  </si>
+  <si>
+    <t>1260.0</t>
+  </si>
+  <si>
+    <t>39541.4</t>
+  </si>
+  <si>
+    <t>39701.4</t>
+  </si>
+  <si>
+    <t>39666.4</t>
   </si>
 </sst>
 </file>
@@ -1213,25 +1459,25 @@
         <v>247</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>241</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
       <c r="G1" t="s">
-        <v>243</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
-        <v>243</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
@@ -1239,16 +1485,25 @@
         <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>250</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -1259,305 +1514,694 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>250</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>251</v>
+        <v>283</v>
       </c>
       <c r="G3" t="s">
-        <v>243</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>243</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>243</v>
+        <v>284</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>253</v>
+        <v>285</v>
       </c>
       <c r="G4" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
       <c r="H4" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>254</v>
+        <v>287</v>
       </c>
       <c r="D5" t="s">
-        <v>255</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
       <c r="G5" t="s">
-        <v>257</v>
+        <v>289</v>
       </c>
       <c r="H5" t="s">
-        <v>257</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>291</v>
       </c>
       <c r="D6" t="s">
-        <v>258</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>257</v>
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>293</v>
       </c>
       <c r="D7" t="s">
-        <v>245</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>260</v>
-      </c>
-      <c r="G7" t="s">
-        <v>261</v>
-      </c>
-      <c r="H7" t="s">
-        <v>261</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>249</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>257</v>
+        <v>295</v>
       </c>
       <c r="D8" t="s">
-        <v>258</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>262</v>
+        <v>296</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>297</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="G9" t="s">
-        <v>261</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>261</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D10" t="s">
-        <v>265</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>266</v>
+        <v>301</v>
       </c>
       <c r="G10" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
       <c r="H10" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>303</v>
       </c>
       <c r="D11" t="s">
-        <v>267</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>268</v>
+        <v>304</v>
       </c>
       <c r="G11" t="s">
-        <v>261</v>
+        <v>305</v>
       </c>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>306</v>
       </c>
       <c r="D12" t="s">
-        <v>269</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="G12" t="s">
-        <v>261</v>
+        <v>308</v>
       </c>
       <c r="H12" t="s">
-        <v>261</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>259</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>309</v>
       </c>
       <c r="D13" t="s">
-        <v>271</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>272</v>
+        <v>310</v>
       </c>
       <c r="G13" t="s">
-        <v>261</v>
+        <v>311</v>
       </c>
       <c r="H13" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>313</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>314</v>
+      </c>
+      <c r="G14" t="s">
+        <v>315</v>
+      </c>
+      <c r="H14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>317</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>318</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>319</v>
+      </c>
+      <c r="G16" t="s">
+        <v>320</v>
+      </c>
+      <c r="H16" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>321</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>322</v>
+      </c>
+      <c r="H17" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
         <v>273</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>274</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C18" t="s">
+        <v>323</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>324</v>
+      </c>
+      <c r="G18" t="s">
+        <v>325</v>
+      </c>
+      <c r="H18" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>326</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>327</v>
+      </c>
+      <c r="G19" t="s">
+        <v>328</v>
+      </c>
+      <c r="H19" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>330</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>331</v>
+      </c>
+      <c r="H20" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>247</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>332</v>
+      </c>
+      <c r="G21" t="s">
+        <v>333</v>
+      </c>
+      <c r="H21" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>249</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>320</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>334</v>
+      </c>
+      <c r="G22" t="s">
+        <v>335</v>
+      </c>
+      <c r="H22" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>249</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>336</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>337</v>
+      </c>
+      <c r="G23" t="s">
+        <v>338</v>
+      </c>
+      <c r="H23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>273</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>339</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>340</v>
+      </c>
+      <c r="G24" t="s">
+        <v>341</v>
+      </c>
+      <c r="H24" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>329</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>342</v>
+      </c>
+      <c r="G25" t="s">
+        <v>343</v>
+      </c>
+      <c r="H25" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>345</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
+        <v>346</v>
+      </c>
+      <c r="G26" t="s">
+        <v>347</v>
+      </c>
+      <c r="H26" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>333</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
         <v>7</v>
       </c>
-      <c r="F14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G14" t="s">
-        <v>261</v>
-      </c>
-      <c r="H14" t="s">
-        <v>261</v>
+      <c r="G27" t="s">
+        <v>349</v>
+      </c>
+      <c r="H27" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>350</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s">
+        <v>352</v>
+      </c>
+      <c r="H28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>273</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>353</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>354</v>
+      </c>
+      <c r="H29" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>355</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" t="s">
+        <v>357</v>
+      </c>
+      <c r="H30" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>